<commit_message>
VAT and PIT proposals, using different scenarios
</commit_message>
<xml_diff>
--- a/Poland_PIT_schedule.xlsx
+++ b/Poland_PIT_schedule.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github\international-tax-competitiveness-index\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32C8C62C-EE49-43A6-84A6-3D83B718C0F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AFCBD03-15C7-4C1D-A408-6AC076CF6E15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{503ABEDA-3C70-4F3A-A48A-3D15830625D4}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{503ABEDA-3C70-4F3A-A48A-3D15830625D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet_2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>Average tax wedge</t>
   </si>
@@ -67,9 +68,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="168" formatCode="_-[$PLN]\ * #,##0.00_-;\-[$PLN]\ * #,##0.00_-;_-[$PLN]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="170" formatCode="_-[$PLN]\ * #,##0_-;\-[$PLN]\ * #,##0_-;_-[$PLN]\ * &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="171" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="_-[$PLN]\ * #,##0.00_-;\-[$PLN]\ * #,##0.00_-;_-[$PLN]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-[$PLN]\ * #,##0_-;\-[$PLN]\ * #,##0_-;_-[$PLN]\ * &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="166" formatCode="0.0%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -117,12 +118,12 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADD01C15-0EA7-4F72-9B60-DB62F8F5F69D}">
   <dimension ref="B2:L9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -504,7 +505,7 @@
       <c r="K3" s="2">
         <v>60000</v>
       </c>
-      <c r="L3">
+      <c r="L3" s="4">
         <v>0</v>
       </c>
     </row>
@@ -588,6 +589,146 @@
       <c r="H9" s="7">
         <f>H6/H7</f>
         <v>2.2705502984928718</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB5F30C9-7AE6-4F8F-AF36-8CA773B5100A}">
+  <dimension ref="B2:L9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="2" width="11.265625" customWidth="1"/>
+    <col min="4" max="5" width="13.53125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.53125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.53125" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" customWidth="1"/>
+    <col min="11" max="11" width="13.53125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="J2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.67</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1.67</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2">
+        <v>30000</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="3">
+        <f>0.67*E4</f>
+        <v>57428.849000000002</v>
+      </c>
+      <c r="E4" s="3">
+        <v>85714.7</v>
+      </c>
+      <c r="F4" s="3">
+        <f>1.67*E4</f>
+        <v>143143.549</v>
+      </c>
+      <c r="J4" s="2">
+        <v>30000</v>
+      </c>
+      <c r="K4" s="2"/>
+      <c r="L4" s="4">
+        <v>0.23499999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0.23499999999999999</v>
+      </c>
+      <c r="H6" s="6">
+        <f>AVERAGE(D6:F6)</f>
+        <v>0.23499999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="5">
+        <f>(($K$3)*$L$3+(D4-$J$4)*$L$4)/D4</f>
+        <v>0.11223939931305257</v>
+      </c>
+      <c r="E7" s="5">
+        <f>(($K$3)*$L$3+(E4-$J$4)*$L$4)/E4</f>
+        <v>0.1527503975397452</v>
+      </c>
+      <c r="F7" s="5">
+        <f>(($K$3)*$L$3+(F4-$J$4)*$L$4)/F4</f>
+        <v>0.18574874104176359</v>
+      </c>
+      <c r="H7" s="6">
+        <f>AVERAGE(D7:F7)</f>
+        <v>0.15024617929818712</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.45">
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ref="D9:F9" si="0">D6/D7</f>
+        <v>2.0937389315898747</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>1.5384575345465381</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="0"/>
+        <v>1.2651498937866976</v>
+      </c>
+      <c r="H9" s="7">
+        <f>H6/H7</f>
+        <v>1.5640996736003889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>